<commit_message>
added faq for french and english
</commit_message>
<xml_diff>
--- a/ESI_PHA_BOT_RESP_BUILDER_FR_CA.xlsx
+++ b/ESI_PHA_BOT_RESP_BUILDER_FR_CA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2243665\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE310CA0-7647-4EA1-B573-A64E003BC241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72154BA6-7E00-49FA-8EC5-67437EAA7151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{1CB3E365-0F38-41A0-882A-60B13BA55A8E}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="56">
   <si>
     <t>RESPONSE_ID</t>
   </si>
@@ -175,13 +175,59 @@
   </si>
   <si>
     <t>Accès refusé. Veuillez vous assurer que vous êtes connecté avec les informations d’identification correctes.</t>
+  </si>
+  <si>
+    <t>ESI_PHA_ORD_INFO_FAQ_WHEN_CHARGED_FOR_ORDER</t>
+  </si>
+  <si>
+    <t>ESI_PHA_ORD_INFO_FAQ_WHERE_TO_FIND_PRESCRIPTION_ID_CARD</t>
+  </si>
+  <si>
+    <t>ESI_PHA_ORD_INFO_FAQ_HOW_TO_CREATE_ONLINE_ACCOUNT</t>
+  </si>
+  <si>
+    <t>ESI_PHA_ORD_INFO_FAQ_HOW_GET_ALL_MY_MEDICATIONS_AT_HOME_DELIVERY</t>
+  </si>
+  <si>
+    <t>ESI_PHA_ORD_INFO_FAQ_WHAT_TEMPERATURE-SENSITIVE_MEDICATION</t>
+  </si>
+  <si>
+    <t>Vous ne serez pas facturé pour votre commande jusqu’à ce que votre médicament soit expédié. Si vous êtes inscrit à notre plan de paiement prolongé, seul le premier paiement sera traité lorsque vos médicaments seront expédiés.
+Pour vérifier l’état de votre commande, vous pouvez vous connecter et aller à Mes médicaments sous Ordonnances. Après vous être connecté, vous pouvez également vérifier s’il existe des moyens d’économiser sur vos médicaments.</t>
+  </si>
+  <si>
+    <t>Nous offrons une carte d’identité numérique à ne pas perdre que vous pouvez conserver avec vous 24/7. Il suffit de le télécharger sur votre téléphone, d’imprimer une copie ou de faire les deux. Vous pouvez même l’enregistrer dans votre portefeuille mobile.
+Comment obtenir votre carte d’identité numérique sur ordonnance :
+En ligne
+Selon votre plan, vous pouvez vous connecter et sélectionner Carte d’identité sur ordonnance sous Compte dans le menu principal. S’il est disponible, vous pouvez imprimer votre carte d’identité d’ordonnance à partir de là. Il suffit de cliquer sur le bouton Télécharger la carte pour télécharger et / ou imprimer votre carte d’identité d’ordonnance.
+Sur l’application mobile Express Scripts®
+Appuyez sur l’icône de menu dans le coin supérieur gauche de votre écran. Allez à Mon dossier et choisissez Carte d’identité sur ordonnance. Vous pouvez utiliser l’application mobile pour afficher votre numéro d’identification d’ordonnance à votre pharmacie ou au cabinet de votre médecin.</t>
+  </si>
+  <si>
+    <t>La création d’un compte Express Scripts en ligne est simple. En seulement quelques minutes, votre compte peut être prêt à partir. Pour vous inscrire, vous pouvez utiliser votre numéro d’ordonnance ou votre numéro de sécurité sociale.
+Une fois que vous avez créé un compte en ligne, vous pouvez :
+Inscrivez-vous aux alertes texte afin de ne jamais manquer une occasion d’enregistrer
+Obtenez des prix transparents sur tous vos médicaments
+Recevez des recommandations d’épargne personnalisées qui retirent les conjectures de votre prestation d’ordonnance
+Transférer des médicaments à notre pharmacie de livraison à domicile
+Rechargez facilement les ordonnances et suivez vos commandes en temps réel
+Et bien plus encore !
+Certaines de ces fonctionnalités peuvent dépendre de votre plan.</t>
+  </si>
+  <si>
+    <t>Pour la plupart, oui ! Express Scripts Pharmacy distribue la plupart des médicaments d’entretien de marque et génériques dans un approvisionnement de 3 mois. Cependant, tout comme les autres pharmacies, nous sommes incapables de stocker tous les médicaments tout le temps.
+Si nous ne transportons pas un certain médicament, si nous manquons d’approvisionnement ou si nous sommes en rupture de stock, nous vous en informerons dès que votre commande sera passée. De plus, votre médecin peut être en mesure de vérifier la disponibilité grâce à l’avantage de prescription en temps réel lors de la prescription, et si votre médicament n’est pas disponible à la livraison à domicile, ils peuvent envoyer l’ordonnance à une pharmacie de détail en réseau de votre choix.</t>
+  </si>
+  <si>
+    <t>Nous expédions vos médicaments dans un emballage inviolable et résistant aux intempéries. Si votre médicament est sensible aux conditions extrêmement chaudes ou froides, nous l’expédions dans un emballage à température contrôlée. Nous calculons soigneusement combien de temps votre commande voyagera et les conditions météorologiques pour nous assurer que nous incluons suffisamment de blocs réfrigérants pour assurer la sécurité de vos médicaments.
+Les médicaments qui nécessitent un contrôle de la température sont envoyés par expédition accélérée sans frais supplémentaires pour vous.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -193,6 +239,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -218,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -229,6 +282,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -563,10 +619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29329887-49B3-45E3-9F81-89EC8C728205}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -734,6 +790,46 @@
       </c>
       <c r="E12" s="5" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="232" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="174" x14ac:dyDescent="0.35">
+      <c r="A15" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="116" x14ac:dyDescent="0.35">
+      <c r="A16" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>